<commit_message>
Subir proyecto de reservar habitacion en pom
</commit_message>
<xml_diff>
--- a/src/test/resources/datadriven/AgenciaDeViajes.xlsx
+++ b/src/test/resources/datadriven/AgenciaDeViajes.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4719F408-6C0A-4796-BEBA-C3C8827D1AFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF9CF14-0765-474D-BF77-5683893BDC70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,7 +13,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -65,17 +65,16 @@
     <t>San Francisco</t>
   </si>
   <si>
-    <t>JANUARY</t>
-  </si>
-  <si>
-    <t>FEBRUARY</t>
+    <t>SEPTEMBER</t>
+  </si>
+  <si>
+    <t>OCTOBER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -120,7 +119,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -133,6 +132,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -422,9 +424,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -442,11 +444,11 @@
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="C2" s="5" t="n">
-        <v>299.0</v>
+      <c r="B2" s="5">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5">
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -457,32 +459,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="2.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="11.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="10.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="11.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="8.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
-    <col min="9" max="10" bestFit="true" customWidth="true" style="2" width="7.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="9.7109375" collapsed="true"/>
-    <col min="12" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="2.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="7.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.140625" style="2" collapsed="1"/>
+    <col min="13" max="13" width="9.140625" style="2"/>
+    <col min="14" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -547,6 +551,9 @@
       <c r="K2" s="4">
         <v>0</v>
       </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="8"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5"/>

</xml_diff>

<commit_message>
Se corrige el error de la automatización al seleccionar el número de habitaciones
</commit_message>
<xml_diff>
--- a/src/test/resources/datadriven/AgenciaDeViajes.xlsx
+++ b/src/test/resources/datadriven/AgenciaDeViajes.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -75,6 +75,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -424,9 +425,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -444,11 +445,11 @@
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
-        <v>14</v>
-      </c>
-      <c r="C2" s="5">
-        <v>299</v>
+      <c r="B2" s="5" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>299.0</v>
       </c>
     </row>
   </sheetData>
@@ -459,7 +460,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
@@ -467,19 +468,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="7.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.140625" style="2" collapsed="1"/>
-    <col min="13" max="13" width="9.140625" style="2"/>
-    <col min="14" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="2.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="12.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="11.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="10.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="11.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="8.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="9" max="10" bestFit="true" customWidth="true" style="2" width="7.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="9.7109375" collapsed="true"/>
+    <col min="12" max="12" style="2" width="9.140625" collapsed="true"/>
+    <col min="13" max="13" style="2" width="9.140625" collapsed="true"/>
+    <col min="14" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>